<commit_message>
intentando arreglar elimina ruta sobrantes
</commit_message>
<xml_diff>
--- a/Reporte Resultados.xlsx
+++ b/Reporte Resultados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Nombre</t>
   </si>
@@ -49,46 +49,19 @@
     <t>A-n32-k5</t>
   </si>
   <si>
-    <t>A-n39-k6</t>
-  </si>
-  <si>
     <t>Set B</t>
   </si>
   <si>
-    <t>B-n31-k5</t>
-  </si>
-  <si>
-    <t>B-n34-k5</t>
-  </si>
-  <si>
-    <t>B-n35-k5</t>
-  </si>
-  <si>
-    <t>B-n38-k6</t>
-  </si>
-  <si>
-    <t>B-n57-k7</t>
-  </si>
-  <si>
-    <t>B-n57-k9</t>
-  </si>
-  <si>
     <t>Set E</t>
   </si>
   <si>
     <t>E-n22-k4</t>
   </si>
   <si>
-    <t>E-n23-k3</t>
-  </si>
-  <si>
-    <t>E-n30-k3</t>
-  </si>
-  <si>
-    <t>E-n33-k4</t>
-  </si>
-  <si>
     <t>Set M</t>
+  </si>
+  <si>
+    <t>Golden</t>
   </si>
 </sst>
 </file>
@@ -427,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -496,33 +469,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" s="1" customFormat="1">
+      <c r="A4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>39</v>
-      </c>
-      <c r="D4">
-        <v>848.182</v>
-      </c>
-      <c r="E4">
-        <v>848.182</v>
-      </c>
-      <c r="F4">
-        <v>848.182</v>
-      </c>
-      <c r="G4">
-        <v>831</v>
-      </c>
-      <c r="H4">
-        <v>2.067629362214207</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1">
@@ -535,299 +484,38 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D6">
-        <v>681.371</v>
+        <v>375.282</v>
       </c>
       <c r="E6">
-        <v>681.371</v>
+        <v>375.2809999999999</v>
       </c>
       <c r="F6">
-        <v>681.371</v>
+        <v>375.282</v>
       </c>
       <c r="G6">
-        <v>672</v>
+        <v>375</v>
       </c>
       <c r="H6">
-        <v>1.394494047619044</v>
+        <v>0.08733333333333367</v>
       </c>
       <c r="I6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
+    <row r="7" spans="1:9" s="1" customFormat="1">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>34</v>
-      </c>
-      <c r="D7">
-        <v>798.253</v>
-      </c>
-      <c r="E7">
-        <v>798.253</v>
-      </c>
-      <c r="F7">
-        <v>798.253</v>
-      </c>
-      <c r="G7">
-        <v>788</v>
-      </c>
-      <c r="H7">
-        <v>1.301142131979693</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1">
+      <c r="A8" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>35</v>
-      </c>
-      <c r="D8">
-        <v>961.7670000000001</v>
-      </c>
-      <c r="E8">
-        <v>961.7435</v>
-      </c>
-      <c r="F8">
-        <v>961.7670000000001</v>
-      </c>
-      <c r="G8">
-        <v>955</v>
-      </c>
-      <c r="H8">
-        <v>0.7061256544502625</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>38</v>
-      </c>
-      <c r="D9">
-        <v>821.069</v>
-      </c>
-      <c r="E9">
-        <v>813.417</v>
-      </c>
-      <c r="F9">
-        <v>821.069</v>
-      </c>
-      <c r="G9">
-        <v>805</v>
-      </c>
-      <c r="H9">
-        <v>1.045590062111801</v>
-      </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>57</v>
-      </c>
-      <c r="D10">
-        <v>1428.039</v>
-      </c>
-      <c r="E10">
-        <v>1368.2185</v>
-      </c>
-      <c r="F10">
-        <v>1428.039</v>
-      </c>
-      <c r="G10">
-        <v>1153</v>
-      </c>
-      <c r="H10">
-        <v>18.66595836947094</v>
-      </c>
-      <c r="I10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
-        <v>9</v>
-      </c>
-      <c r="C11">
-        <v>57</v>
-      </c>
-      <c r="D11">
-        <v>1636.607</v>
-      </c>
-      <c r="E11">
-        <v>1636.607</v>
-      </c>
-      <c r="F11">
-        <v>1636.607</v>
-      </c>
-      <c r="G11">
-        <v>1598</v>
-      </c>
-      <c r="H11">
-        <v>2.415957446808514</v>
-      </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>22</v>
-      </c>
-      <c r="D13">
-        <v>375.28</v>
-      </c>
-      <c r="E13">
-        <v>375.28</v>
-      </c>
-      <c r="F13">
-        <v>375.28</v>
-      </c>
-      <c r="G13">
-        <v>375</v>
-      </c>
-      <c r="H13">
-        <v>0.07466666666666733</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>23</v>
-      </c>
-      <c r="D14">
-        <v>569.746</v>
-      </c>
-      <c r="E14">
-        <v>569.746</v>
-      </c>
-      <c r="F14">
-        <v>569.746</v>
-      </c>
-      <c r="G14">
-        <v>569</v>
-      </c>
-      <c r="H14">
-        <v>0.1311072056239038</v>
-      </c>
-      <c r="I14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>30</v>
-      </c>
-      <c r="D15">
-        <v>670.485</v>
-      </c>
-      <c r="E15">
-        <v>594.8928</v>
-      </c>
-      <c r="F15">
-        <v>670.485</v>
-      </c>
-      <c r="G15">
-        <v>534</v>
-      </c>
-      <c r="H15">
-        <v>11.40314606741573</v>
-      </c>
-      <c r="I15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="C16">
-        <v>33</v>
-      </c>
-      <c r="D16">
-        <v>852.439</v>
-      </c>
-      <c r="E16">
-        <v>852.439</v>
-      </c>
-      <c r="F16">
-        <v>852.439</v>
-      </c>
-      <c r="G16">
-        <v>835</v>
-      </c>
-      <c r="H16">
-        <v>2.088502994011976</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="1" customFormat="1">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>